<commit_message>
Version 1.1.0: Real-time progress tracking, SSE implementation, and comprehensive documentation
</commit_message>
<xml_diff>
--- a/test_questions.xlsx
+++ b/test_questions.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,35 +424,21 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>What is your age?</t>
+          <t>Encuesta</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>How satisfied are you with our service?</t>
+          <t>&lt;i&gt;Seleccione una opción&lt;/i&gt;</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Would you recommend us to others?</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>What is your favorite color?</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>How often do you use our product?</t>
+          <t>&lt;em&gt;Seleccione todas las opciones que correspondan&lt;/em&gt;</t>
         </is>
       </c>
     </row>

</xml_diff>